<commit_message>
Started analysis from AST
</commit_message>
<xml_diff>
--- a/tools/timing/data.xlsx
+++ b/tools/timing/data.xlsx
@@ -14,7 +14,8 @@
     <sheet name="Unraveling" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Merging" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Compare" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Float numbers multiplication" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="mem cycle" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Float numbers multiplication" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="52">
   <si>
     <t xml:space="preserve">Matrix Size 5</t>
   </si>
@@ -158,6 +159,12 @@
   </si>
   <si>
     <t xml:space="preserve">Matrix Matrix Multiplication (float)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column Wise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL</t>
   </si>
   <si>
     <t xml:space="preserve">Multiplication</t>
@@ -378,7 +385,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -446,10 +453,13 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -457,10 +467,13 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -468,10 +481,13 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -479,10 +495,13 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -490,10 +509,13 @@
             <c:idx val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -501,10 +523,13 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -512,10 +537,13 @@
             <c:idx val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -523,10 +551,13 @@
             <c:idx val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -534,10 +565,13 @@
             <c:idx val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -545,10 +579,13 @@
             <c:idx val="9"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -556,10 +593,13 @@
             <c:idx val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -567,10 +607,13 @@
             <c:idx val="11"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -578,10 +621,13 @@
             <c:idx val="12"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -589,10 +635,13 @@
             <c:idx val="13"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -600,10 +649,13 @@
             <c:idx val="14"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -868,11 +920,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="35804739"/>
-        <c:axId val="24487779"/>
+        <c:axId val="34854988"/>
+        <c:axId val="13768869"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35804739"/>
+        <c:axId val="34854988"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,14 +960,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24487779"/>
+        <c:crossAx val="13768869"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24487779"/>
+        <c:axId val="13768869"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +1010,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35804739"/>
+        <c:crossAx val="34854988"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -996,7 +1048,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1064,10 +1116,13 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1075,10 +1130,13 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1086,10 +1144,13 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1097,10 +1158,13 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1108,10 +1172,13 @@
             <c:idx val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1119,10 +1186,13 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1130,10 +1200,13 @@
             <c:idx val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1141,10 +1214,13 @@
             <c:idx val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1152,10 +1228,13 @@
             <c:idx val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1163,10 +1242,13 @@
             <c:idx val="9"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1174,10 +1256,13 @@
             <c:idx val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1185,10 +1270,13 @@
             <c:idx val="11"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1196,10 +1284,13 @@
             <c:idx val="12"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1207,10 +1298,13 @@
             <c:idx val="13"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1218,10 +1312,13 @@
             <c:idx val="14"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1229,10 +1326,13 @@
             <c:idx val="15"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1240,10 +1340,13 @@
             <c:idx val="16"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1251,10 +1354,13 @@
             <c:idx val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1262,10 +1368,13 @@
             <c:idx val="18"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1273,10 +1382,13 @@
             <c:idx val="19"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1284,10 +1396,13 @@
             <c:idx val="20"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1295,10 +1410,13 @@
             <c:idx val="21"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1668,11 +1786,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="69139071"/>
-        <c:axId val="58912524"/>
+        <c:axId val="45356592"/>
+        <c:axId val="48595503"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69139071"/>
+        <c:axId val="45356592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,14 +1826,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58912524"/>
+        <c:crossAx val="48595503"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58912524"/>
+        <c:axId val="48595503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1758,7 +1876,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69139071"/>
+        <c:crossAx val="45356592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1796,7 +1914,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1864,10 +1982,13 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1875,10 +1996,13 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1886,10 +2010,13 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1897,10 +2024,13 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1908,10 +2038,13 @@
             <c:idx val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1919,10 +2052,13 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1930,10 +2066,13 @@
             <c:idx val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1941,10 +2080,13 @@
             <c:idx val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1952,10 +2094,13 @@
             <c:idx val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1963,10 +2108,13 @@
             <c:idx val="9"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1974,10 +2122,13 @@
             <c:idx val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1985,10 +2136,13 @@
             <c:idx val="11"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -1996,10 +2150,13 @@
             <c:idx val="12"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2007,10 +2164,13 @@
             <c:idx val="13"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2018,10 +2178,13 @@
             <c:idx val="14"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2029,10 +2192,13 @@
             <c:idx val="15"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2040,10 +2206,13 @@
             <c:idx val="16"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2051,10 +2220,13 @@
             <c:idx val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2062,10 +2234,13 @@
             <c:idx val="18"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2073,10 +2248,13 @@
             <c:idx val="19"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2084,10 +2262,13 @@
             <c:idx val="20"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2095,10 +2276,13 @@
             <c:idx val="21"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2106,10 +2290,13 @@
             <c:idx val="22"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2117,10 +2304,13 @@
             <c:idx val="23"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2128,10 +2318,13 @@
             <c:idx val="24"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2139,10 +2332,13 @@
             <c:idx val="25"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2150,10 +2346,13 @@
             <c:idx val="26"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2161,10 +2360,13 @@
             <c:idx val="27"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2172,10 +2374,13 @@
             <c:idx val="28"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2183,10 +2388,13 @@
             <c:idx val="29"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2194,10 +2402,13 @@
             <c:idx val="30"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2205,10 +2416,13 @@
             <c:idx val="31"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2216,10 +2430,13 @@
             <c:idx val="32"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2227,10 +2444,13 @@
             <c:idx val="33"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2238,10 +2458,13 @@
             <c:idx val="34"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2249,10 +2472,13 @@
             <c:idx val="35"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2260,10 +2486,13 @@
             <c:idx val="36"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2271,10 +2500,13 @@
             <c:idx val="37"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2282,10 +2514,13 @@
             <c:idx val="38"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2293,10 +2528,13 @@
             <c:idx val="39"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2304,10 +2542,13 @@
             <c:idx val="40"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2315,10 +2556,13 @@
             <c:idx val="41"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2326,10 +2570,13 @@
             <c:idx val="42"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2337,10 +2584,13 @@
             <c:idx val="43"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2348,10 +2598,13 @@
             <c:idx val="44"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2359,10 +2612,13 @@
             <c:idx val="45"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2370,10 +2626,13 @@
             <c:idx val="46"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2381,10 +2640,13 @@
             <c:idx val="47"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2392,10 +2654,13 @@
             <c:idx val="48"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2403,10 +2668,13 @@
             <c:idx val="49"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2414,10 +2682,13 @@
             <c:idx val="50"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2425,10 +2696,13 @@
             <c:idx val="51"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2436,10 +2710,13 @@
             <c:idx val="52"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2447,10 +2724,13 @@
             <c:idx val="53"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2458,10 +2738,13 @@
             <c:idx val="54"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2469,10 +2752,13 @@
             <c:idx val="55"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2480,10 +2766,13 @@
             <c:idx val="56"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln w="1772368920">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2491,10 +2780,13 @@
             <c:idx val="57"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2502,10 +2794,13 @@
             <c:idx val="58"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2513,10 +2808,13 @@
             <c:idx val="59"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1"/>
-              </a:solidFill>
-              <a:ln w="12240360">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2524,10 +2822,13 @@
             <c:idx val="60"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2535,10 +2836,13 @@
             <c:idx val="61"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2546,10 +2850,13 @@
             <c:idx val="62"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2557,10 +2864,13 @@
             <c:idx val="63"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2568,10 +2878,13 @@
             <c:idx val="64"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2579,10 +2892,13 @@
             <c:idx val="65"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -2590,10 +2906,13 @@
             <c:idx val="66"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:ln w="28440">
+                <a:solidFill>
+                  <a:srgbClr val="ed7d31"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -3638,11 +3957,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="94817520"/>
-        <c:axId val="6218155"/>
+        <c:axId val="55614871"/>
+        <c:axId val="89378099"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94817520"/>
+        <c:axId val="55614871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3678,14 +3997,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6218155"/>
+        <c:crossAx val="89378099"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6218155"/>
+        <c:axId val="89378099"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3728,7 +4047,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94817520"/>
+        <c:crossAx val="55614871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3771,15 +4090,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>414360</xdr:colOff>
+      <xdr:colOff>415080</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>641160</xdr:colOff>
+      <xdr:colOff>640440</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3787,8 +4106,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8615160" y="195120"/>
-        <a:ext cx="4722480" cy="2923200"/>
+        <a:off x="8873280" y="195120"/>
+        <a:ext cx="4873320" cy="2922480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3801,15 +4120,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4680</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>231480</xdr:colOff>
+      <xdr:colOff>230760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3817,8 +4136,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8205480" y="4263480"/>
-        <a:ext cx="4722480" cy="3063960"/>
+        <a:off x="8463600" y="4264200"/>
+        <a:ext cx="4873320" cy="3061800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3831,15 +4150,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>15120</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>865800</xdr:colOff>
+      <xdr:colOff>864360</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3847,8 +4166,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8215200" y="8764200"/>
-        <a:ext cx="6471360" cy="3516840"/>
+        <a:off x="8473320" y="8764920"/>
+        <a:ext cx="6659280" cy="3515400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3868,19 +4187,19 @@
   </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4741,11 +5060,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5008,10 +5327,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="13.0688259109312"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6350,11 +6669,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6587,14 +6906,14 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6761133603239"/>
@@ -6964,17 +7283,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.6072874493927"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.10526315789474"/>
@@ -6984,11 +7303,14 @@
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="0"/>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -7009,6 +7331,7 @@
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -7032,6 +7355,7 @@
         <f aca="false">E3/D3*100</f>
         <v>-8.91850683774992</v>
       </c>
+      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -7055,6 +7379,7 @@
         <f aca="false">E4/D4*100</f>
         <v>-8.9084859721242</v>
       </c>
+      <c r="G4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
@@ -7063,6 +7388,7 @@
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -7073,6 +7399,7 @@
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -7093,6 +7420,7 @@
       <c r="F7" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="G7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -7116,6 +7444,7 @@
         <f aca="false">E8/D8*100</f>
         <v>7.0628774283873</v>
       </c>
+      <c r="G8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -7139,11 +7468,27 @@
         <f aca="false">E9/D9*100</f>
         <v>7.1819658741058</v>
       </c>
+      <c r="G9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -7164,6 +7509,7 @@
       <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="G12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -7187,6 +7533,7 @@
         <f aca="false">E13/D13*100</f>
         <v>9.02719560423539</v>
       </c>
+      <c r="G13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -7210,6 +7557,7 @@
         <f aca="false">E14/D14*100</f>
         <v>8.94124881098708</v>
       </c>
+      <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -7232,6 +7580,268 @@
       <c r="F15" s="1" t="n">
         <f aca="false">E15/D15*100</f>
         <v>9.17861174405744</v>
+      </c>
+      <c r="G15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>253773</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>4943.96</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">C21*48</f>
+        <v>237310.08</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">B21-D21</f>
+        <v>16462.92</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">E21/D21*100</f>
+        <v>6.93730329533411</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <f aca="false">148565+400*20+400+20</f>
+        <v>156985</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>849853</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>16586.23</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <f aca="false">C22*48</f>
+        <v>796139.04</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <f aca="false">B22-D22</f>
+        <v>53713.96</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">E22/D22*100</f>
+        <v>6.74680643722734</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>2006733</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>39199.43</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">C23*48</f>
+        <v>1881572.64</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">B23-D23</f>
+        <v>125160.36</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <f aca="false">E23/D23*100</f>
+        <v>6.65190157101775</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>152182</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>2833.54</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">C29*48</f>
+        <v>136009.92</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <f aca="false">B29-D29</f>
+        <v>16172.08</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <f aca="false">E29/D29*100</f>
+        <v>11.8903679966873</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>504262</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>9388.69</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">C30*48</f>
+        <v>450657.12</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <f aca="false">B30-D30</f>
+        <v>53604.88</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <f aca="false">E30/D30*100</f>
+        <v>11.8948259377329</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>1184342</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>22048.76</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">C31*48</f>
+        <v>1058340.48</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">B31-D31</f>
+        <v>126001.52</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <f aca="false">E31/D31*100</f>
+        <v>11.9055750376287</v>
       </c>
     </row>
   </sheetData>
@@ -7250,141 +7860,412 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1821862348178"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>46</v>
+        <v>189370</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>4943.96</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">C3*48</f>
+        <v>237310.08</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">B3-D3</f>
+        <v>-47940.08</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">E3/D3*100</f>
+        <v>-20.2014511983646</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>440</v>
+        <v>632950</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>16586.23</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">C4*48</f>
+        <v>796139.04</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">B4-D4</f>
+        <v>-163189.04</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <f aca="false">E4/D4*100</f>
+        <v>-20.4975553013956</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>4459</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>44586</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>4.4586</v>
+        <v>1493130</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>39199.43</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="false">C5*48</f>
+        <v>1881572.64</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">B5-D5</f>
+        <v>-388442.64</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <f aca="false">E5/D5*100</f>
+        <v>-20.64457314813</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <f aca="false">48*B8</f>
-        <v>214.0128</v>
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>49</v>
+      <c r="A11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>143770</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2833.54</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">C11*48</f>
+        <v>136009.92</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">B11-D11</f>
+        <v>7760.08000000002</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">E11/D11*100</f>
+        <v>5.70552500876408</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
+      <c r="A12" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>476350</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>9388.69</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">C12*48</f>
+        <v>450657.12</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">B12-D12</f>
+        <v>25692.88</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <f aca="false">E12/D12*100</f>
+        <v>5.70120361129544</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>2597</v>
+        <v>1118730</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>22048.76</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">C13*48</f>
+        <v>1058340.48</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">B13-D13</f>
+        <v>60389.52</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">E13/D13*100</f>
+        <v>5.70605784633694</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>25959</v>
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>2.5959</v>
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>48</v>
+      <c r="A19" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="n">
-        <f aca="false">B18*48</f>
-        <v>124.6032</v>
+        <v>189771</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>4943.96</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">C19*48</f>
+        <v>237310.08</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">B19-D19</f>
+        <v>-47539.08</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">E19/D19*100</f>
+        <v>-20.032473968236</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>633851</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>16586.23</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">C20*48</f>
+        <v>796139.04</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">B20-D20</f>
+        <v>-162288.04</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <f aca="false">E20/D20*100</f>
+        <v>-20.384384114614</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1494731</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>39199.43</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">C21*48</f>
+        <v>1881572.64</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">B21-D21</f>
+        <v>-386841.64</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">E21/D21*100</f>
+        <v>-20.5594847510113</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>144171</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>2833.54</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">C27*48</f>
+        <v>136009.92</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <f aca="false">B27-D27</f>
+        <v>8161.08000000002</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <f aca="false">E27/D27*100</f>
+        <v>6.00035644458876</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>477251</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>9388.69</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">C28*48</f>
+        <v>450657.12</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <f aca="false">B28-D28</f>
+        <v>26593.88</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <f aca="false">E28/D28*100</f>
+        <v>5.90113388200768</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>1120331</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>22048.76</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">C29*48</f>
+        <v>1058340.48</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <f aca="false">B29-D29</f>
+        <v>61990.52</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <f aca="false">E29/D29*100</f>
+        <v>5.85733241536788</v>
       </c>
     </row>
   </sheetData>
@@ -7396,4 +8277,171 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4459</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>44586</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>4.4586</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <f aca="false">48*B8</f>
+        <v>214.0128</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>25959</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>2.5959</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <f aca="false">B18*48</f>
+        <v>124.6032</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>